<commit_message>
Update Controller, View And Model For Admin
</commit_message>
<xml_diff>
--- a/Excel/LaporanKeuangan/laporan_keuangan.xlsx
+++ b/Excel/LaporanKeuangan/laporan_keuangan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Laporan Keuangan Toko AnnisaATK</t>
   </si>
@@ -26,10 +26,7 @@
     <t>Keuntungan</t>
   </si>
   <si>
-    <t>2023-06-25</t>
-  </si>
-  <si>
-    <t>2023-06-26</t>
+    <t>2023-07-11</t>
   </si>
   <si>
     <t>Total</t>
@@ -412,7 +409,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:B1"/>
@@ -443,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>6620</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -451,15 +448,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>3520</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>10140</v>
+        <v>4000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>